<commit_message>
Assignment 6 - Question 3, Question 6 completed. Question 7 in progress
</commit_message>
<xml_diff>
--- a/Assignment 6 CIELAB/TwoDegChromaticity.xlsx
+++ b/Assignment 6 CIELAB/TwoDegChromaticity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pratheepkumarc/Documents/Development/Matlab/Principles-of-Color-Science/Assignment 6 CIELAB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D849D4-2E1B-DF4C-A4C0-58074B1A59AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDFD31BB-487D-1A43-BF5A-3F9DE6495B43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -438,8 +438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83:XFD83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>